<commit_message>
excel update suite 1 and 4
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -1072,7 +1072,7 @@
   <dimension ref="A1:AMK32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="E3" s="6">
         <f>IF(B3="Y",COUNTIF(Suite1!B2:B50,"Y"),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1172,7 +1172,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>9</v>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="E6" s="6">
         <f>IF(B6="Y",COUNTIF(Suite4!B2:B50,"Y"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1430,7 +1430,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1475,7 +1475,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>43</v>
@@ -2150,7 +2150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2220,7 +2222,7 @@
         <v>153</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>154</v>

</xml_diff>